<commit_message>
Adjusted image output and fixed save/export bugs
</commit_message>
<xml_diff>
--- a/assets/resources/tool_database.xlsx
+++ b/assets/resources/tool_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deleum-my.sharepoint.com/personal/adam_mohdtaufik_deleum_com/Documents/Documents/ToolStringEditor/assets/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1813" documentId="8_{3731B2D3-2851-4964-AE06-C382F04C3BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B34E248-3E80-42B9-8DD6-7F0FEBB3E50A}"/>
+  <xr:revisionPtr revIDLastSave="1822" documentId="8_{3731B2D3-2851-4964-AE06-C382F04C3BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2353860A-4BE2-4332-B304-7A18231DE0EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1389,9 +1389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="84" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I298" sqref="I298"/>
+      <selection pane="topRight" activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6197,7 +6197,7 @@
         <v>1.875</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>60</v>
@@ -6271,7 +6271,7 @@
         <v>1.875</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F136" s="3" t="s">
         <v>59</v>
@@ -6345,7 +6345,7 @@
         <v>2.5</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>59</v>
+        <v>229</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>59</v>
@@ -6382,7 +6382,7 @@
         <v>2.5</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>229</v>
+        <v>59</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>229</v>
@@ -9310,7 +9310,7 @@
         <v>1.6875</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>68</v>
+        <v>279</v>
       </c>
       <c r="F246" s="3" t="s">
         <v>68</v>
@@ -9341,7 +9341,7 @@
         <v>1.6875</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F247" s="3" t="s">
         <v>280</v>
@@ -9372,7 +9372,7 @@
         <v>1.6875</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>60</v>
+        <v>279</v>
       </c>
       <c r="F248" s="3" t="s">
         <v>60</v>
@@ -9403,7 +9403,7 @@
         <v>1.6875</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>242</v>
+        <v>279</v>
       </c>
       <c r="F249" s="3" t="s">
         <v>242</v>
@@ -10966,7 +10966,7 @@
         <v>1.6875</v>
       </c>
       <c r="E301" s="3" t="s">
-        <v>280</v>
+        <v>68</v>
       </c>
       <c r="F301" s="3" t="s">
         <v>280</v>

</xml_diff>